<commit_message>
update archetype spreadsheet to get the proper location of the windows on left and right of the house
update entries for left and right windows in options file for BC-LEEP
</commit_message>
<xml_diff>
--- a/OptFramework/MODEL-work/LEEP_BC_model_geometry.xlsx
+++ b/OptFramework/MODEL-work/LEEP_BC_model_geometry.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6135" windowWidth="19230" windowHeight="5940"/>
+    <workbookView xWindow="-15" yWindow="6135" windowWidth="19230" windowHeight="5940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry options" sheetId="4" r:id="rId1"/>
@@ -1722,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2296,7 +2296,7 @@
         <v>2.77</v>
       </c>
       <c r="Q10" s="88">
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
       <c r="R10" s="88">
         <v>0</v>
@@ -2323,15 +2323,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.7109375" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -2438,7 +2438,7 @@
       </c>
       <c r="J6" s="33">
         <f>+(INDEX(x2nd,2)-INDEX(x2nd,1))*(INDEX(z2nd,7)-INDEX(z2nd,2))</f>
-        <v>19.94408</v>
+        <v>19.944079999999996</v>
       </c>
       <c r="K6" s="33">
         <f>+(INDEX(x3rd,2)-INDEX(x3rd,1))*(INDEX(z3rd,7)-INDEX(z3rd,2))</f>
@@ -2474,7 +2474,7 @@
       </c>
       <c r="J7" s="33">
         <f>+(INDEX(y2nd,3)-INDEX(y2nd,2))*(INDEX(z2nd,7)-(INDEX(z2nd,3)))</f>
-        <v>28.245810619826369</v>
+        <v>28.245810619826365</v>
       </c>
       <c r="K7" s="33">
         <f>+(INDEX(y3rd,3)-INDEX(y3rd,2))*(INDEX(z3rd,7)-(INDEX(z3rd,3)))</f>
@@ -2510,7 +2510,7 @@
       </c>
       <c r="J8" s="33">
         <f>(INDEX(x2nd,3)-INDEX(x2nd,4))*(INDEX(z2nd,7)-INDEX(z2nd,4))</f>
-        <v>19.94408</v>
+        <v>19.944079999999996</v>
       </c>
       <c r="K8" s="33">
         <f>(INDEX(x3rd,3)-INDEX(x3rd,4))*(INDEX(z3rd,7)-INDEX(z3rd,4))</f>
@@ -2547,7 +2547,7 @@
       </c>
       <c r="J9" s="33">
         <f>(INDEX(y2nd,4)-INDEX(y2nd,1))*(INDEX(z2nd,8)-INDEX(z2nd,4))</f>
-        <v>28.245810619826369</v>
+        <v>28.245810619826365</v>
       </c>
       <c r="K9" s="33">
         <f>(INDEX(y3rd,4)-INDEX(y3rd,1))*(INDEX(z3rd,8)-INDEX(z3rd,4))</f>
@@ -2659,11 +2659,11 @@
       </c>
       <c r="J12" s="15">
         <f>AreaWall1_2nd*AreaWinWall1Ratio/100</f>
-        <v>4.3876976000000001</v>
+        <v>4.3876975999999992</v>
       </c>
       <c r="K12" s="15">
         <f>+IF(NumStoreys=3,AreaWall1_2nd*AreaWinWall1Ratio/100,0)</f>
-        <v>4.3876976000000001</v>
+        <v>4.3876975999999992</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>0</v>
@@ -2688,7 +2688,7 @@
       <c r="B13" s="7"/>
       <c r="C13" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!$B$3:$U$38,16,FALSE)</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>1</v>
@@ -2709,11 +2709,11 @@
       </c>
       <c r="J13" s="17">
         <f>AreaWall2_2nd*AreaWinWall2Ratio/100</f>
-        <v>3.9544134867756919</v>
+        <v>3.954413486775691</v>
       </c>
       <c r="K13" s="17">
         <f>+IF(NumStoreys=3,AreaWall2_2nd*AreaWinWall2Ratio/100,0)</f>
-        <v>3.9544134867756919</v>
+        <v>3.954413486775691</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>0</v>
@@ -2759,11 +2759,11 @@
       </c>
       <c r="J14" s="18">
         <f>AreaWall3_2nd*AreaWinWall3Ratio/100</f>
-        <v>4.5871383999999997</v>
+        <v>4.5871383999999988</v>
       </c>
       <c r="K14" s="18">
         <f>+IF(NumStoreys=3,AreaWall3_2nd*AreaWinWall3Ratio/100,0)</f>
-        <v>4.5871383999999997</v>
+        <v>4.5871383999999988</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>0</v>
@@ -2788,7 +2788,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="39">
         <f>Hght_Flr1+Opt_Bsm_Height</f>
-        <v>2.72</v>
+        <v>5.1584000000000003</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>49</v>
@@ -2854,7 +2854,7 @@
       </c>
       <c r="C17" s="35">
         <f>Opt_Main_Height+Hght_Flr2+Hght_Flr3+(Opt_Roof_Peak_W*Roof_Slope1)</f>
-        <v>10.161</v>
+        <v>12.599399999999999</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
@@ -2961,7 +2961,7 @@
       </c>
       <c r="I24" s="90">
         <f>+SUM(J6:J9)-SUM(J12:J15)</f>
-        <v>83.450249294770856</v>
+        <v>83.450249294770828</v>
       </c>
       <c r="J24" t="s">
         <v>0</v>
@@ -3003,7 +3003,7 @@
       </c>
       <c r="I26">
         <f>2*(Opt_Width*Opt_Bsm_Height)+2*(Opt_Length*Opt_Bsm_Height)</f>
-        <v>0</v>
+        <v>77.81869489230769</v>
       </c>
       <c r="J26" t="s">
         <v>0</v>
@@ -3154,7 +3154,7 @@
       </c>
       <c r="D36" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
       <c r="F36" s="24">
         <v>0</v>
@@ -3164,7 +3164,7 @@
       </c>
       <c r="H36" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>2.72</v>
+        <v>5.1584000000000003</v>
       </c>
       <c r="J36" s="24">
         <v>0</v>
@@ -3174,7 +3174,7 @@
       </c>
       <c r="L36" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
-        <v>5.74</v>
+        <v>8.1783999999999999</v>
       </c>
       <c r="N36" s="24">
         <v>0</v>
@@ -3184,7 +3184,7 @@
       </c>
       <c r="P36" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
       <c r="R36" s="24">
         <v>0</v>
@@ -3209,7 +3209,7 @@
       </c>
       <c r="D37" s="24">
         <f>Opt_Bsm_Height</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
       <c r="F37" s="25">
         <f>Opt_Width</f>
@@ -3220,7 +3220,7 @@
       </c>
       <c r="H37" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>2.72</v>
+        <v>5.1584000000000003</v>
       </c>
       <c r="J37" s="25">
         <f>Opt_Width</f>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="L37" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
-        <v>5.74</v>
+        <v>8.1783999999999999</v>
       </c>
       <c r="N37" s="25">
         <f>Opt_Width</f>
@@ -3242,7 +3242,7 @@
       </c>
       <c r="P37" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
       <c r="R37" s="25">
         <f>Opt_Width</f>
@@ -3269,7 +3269,7 @@
       </c>
       <c r="D38" s="24">
         <f>Opt_Bsm_Height</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
       <c r="F38" s="25">
         <f>Opt_Width</f>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="H38" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>2.72</v>
+        <v>5.1584000000000003</v>
       </c>
       <c r="J38" s="25">
         <f>Opt_Width</f>
@@ -3293,7 +3293,7 @@
       </c>
       <c r="L38" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
-        <v>5.74</v>
+        <v>8.1783999999999999</v>
       </c>
       <c r="N38" s="25">
         <f>Opt_Width</f>
@@ -3305,7 +3305,7 @@
       </c>
       <c r="P38" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
       <c r="R38" s="25">
         <f>Opt_Width</f>
@@ -3332,7 +3332,7 @@
       </c>
       <c r="D39" s="24">
         <f>Opt_Bsm_Height</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
       <c r="F39" s="24">
         <v>0</v>
@@ -3343,7 +3343,7 @@
       </c>
       <c r="H39" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>2.72</v>
+        <v>5.1584000000000003</v>
       </c>
       <c r="J39" s="24">
         <v>0</v>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="L39" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
-        <v>5.74</v>
+        <v>8.1783999999999999</v>
       </c>
       <c r="N39" s="24">
         <v>0</v>
@@ -3365,7 +3365,7 @@
       </c>
       <c r="P39" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
       <c r="R39" s="24">
         <v>0</v>
@@ -3390,7 +3390,7 @@
       </c>
       <c r="D40" s="24">
         <f>Opt_Main_Height</f>
-        <v>2.72</v>
+        <v>5.1584000000000003</v>
       </c>
       <c r="F40" s="24">
         <v>0</v>
@@ -3400,7 +3400,7 @@
       </c>
       <c r="H40" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>5.74</v>
+        <v>8.1783999999999999</v>
       </c>
       <c r="J40" s="24">
         <v>0</v>
@@ -3410,7 +3410,7 @@
       </c>
       <c r="L40" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
       <c r="N40" s="25">
         <f>+Opt_Roof_Peak_W</f>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="P40" s="24">
         <f>+C17</f>
-        <v>10.161</v>
+        <v>12.599399999999999</v>
       </c>
       <c r="R40" s="24">
         <v>0</v>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="T40" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
@@ -3447,7 +3447,7 @@
       </c>
       <c r="D41" s="24">
         <f>Opt_Main_Height</f>
-        <v>2.72</v>
+        <v>5.1584000000000003</v>
       </c>
       <c r="F41" s="25">
         <f>Opt_Width</f>
@@ -3458,7 +3458,7 @@
       </c>
       <c r="H41" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>5.74</v>
+        <v>8.1783999999999999</v>
       </c>
       <c r="J41" s="25">
         <f>Opt_Width</f>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="L41" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
       <c r="N41" s="25">
         <f>+Opt_Roof_Peak_W</f>
@@ -3481,7 +3481,7 @@
       </c>
       <c r="P41" s="24">
         <f>+C17</f>
-        <v>10.161</v>
+        <v>12.599399999999999</v>
       </c>
       <c r="R41" s="25">
         <f>Opt_Width</f>
@@ -3492,7 +3492,7 @@
       </c>
       <c r="T41" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="D42" s="24">
         <f>Opt_Main_Height</f>
-        <v>2.72</v>
+        <v>5.1584000000000003</v>
       </c>
       <c r="F42" s="25">
         <f>Opt_Width</f>
@@ -3521,7 +3521,7 @@
       </c>
       <c r="H42" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>5.74</v>
+        <v>8.1783999999999999</v>
       </c>
       <c r="J42" s="25">
         <f>Opt_Width</f>
@@ -3533,7 +3533,7 @@
       </c>
       <c r="L42" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
       <c r="N42" s="83"/>
       <c r="O42" s="84"/>
@@ -3547,7 +3547,7 @@
       </c>
       <c r="T42" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="D43" s="24">
         <f>Opt_Main_Height</f>
-        <v>2.72</v>
+        <v>5.1584000000000003</v>
       </c>
       <c r="F43" s="24">
         <v>0</v>
@@ -3574,7 +3574,7 @@
       </c>
       <c r="H43" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>5.74</v>
+        <v>8.1783999999999999</v>
       </c>
       <c r="J43" s="24">
         <v>0</v>
@@ -3585,7 +3585,7 @@
       </c>
       <c r="L43" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
       <c r="N43" s="84"/>
       <c r="O43" s="84"/>
@@ -3598,7 +3598,7 @@
       </c>
       <c r="T43" s="57">
         <f>Opt_Bsm_Height</f>
-        <v>0</v>
+        <v>2.4384000000000001</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
@@ -3615,7 +3615,7 @@
       </c>
       <c r="D44" s="26">
         <f>INDEX(z1st,1)+0.5</f>
-        <v>0.5</v>
+        <v>2.9384000000000001</v>
       </c>
       <c r="F44" s="26">
         <f>INDEX(x2nd,1)+0.5</f>
@@ -3627,7 +3627,7 @@
       </c>
       <c r="H44" s="26">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>3.22</v>
+        <v>5.6584000000000003</v>
       </c>
       <c r="J44" s="26">
         <f>INDEX(x3rd,1)+0.5</f>
@@ -3639,7 +3639,7 @@
       </c>
       <c r="L44" s="26">
         <f>INDEX(z3rd,1)+0.5</f>
-        <v>6.24</v>
+        <v>8.6783999999999999</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
@@ -3656,7 +3656,7 @@
       </c>
       <c r="D45" s="26">
         <f>INDEX(z1st,1)+0.5</f>
-        <v>0.5</v>
+        <v>2.9384000000000001</v>
       </c>
       <c r="F45" s="27">
         <f>INDEX(x2nd,9)+Len_WinWall1</f>
@@ -3668,7 +3668,7 @@
       </c>
       <c r="H45" s="26">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>3.22</v>
+        <v>5.6584000000000003</v>
       </c>
       <c r="J45" s="27">
         <f>INDEX(x3rd,9)+Len_WinWall1</f>
@@ -3680,7 +3680,7 @@
       </c>
       <c r="L45" s="26">
         <f>INDEX(z3rd,1)+0.5</f>
-        <v>6.24</v>
+        <v>8.6783999999999999</v>
       </c>
       <c r="N45" s="96" t="s">
         <v>181</v>
@@ -3702,7 +3702,7 @@
       </c>
       <c r="D46" s="26">
         <f>INDEX(z1st,9)+Hght_WinWall1</f>
-        <v>1.86</v>
+        <v>4.2984</v>
       </c>
       <c r="F46" s="27">
         <f>INDEX(x2nd,9)+Len_WinWall1</f>
@@ -3714,7 +3714,7 @@
       </c>
       <c r="H46" s="26">
         <f>INDEX(z2nd,9)+Hght_WinWall1</f>
-        <v>4.58</v>
+        <v>7.0184000000000006</v>
       </c>
       <c r="J46" s="27">
         <f>INDEX(x3rd,9)+Len_WinWall1</f>
@@ -3726,7 +3726,7 @@
       </c>
       <c r="L46" s="26">
         <f>INDEX(z3rd,9)+Hght_WinWall1</f>
-        <v>7.6000000000000005</v>
+        <v>10.038399999999999</v>
       </c>
       <c r="N46" s="91" t="s">
         <v>2</v>
@@ -3752,7 +3752,7 @@
       </c>
       <c r="D47" s="26">
         <f>INDEX(z1st,10)+Hght_WinWall1</f>
-        <v>1.86</v>
+        <v>4.2984</v>
       </c>
       <c r="F47" s="26">
         <f>INDEX(x2nd,9)</f>
@@ -3764,7 +3764,7 @@
       </c>
       <c r="H47" s="26">
         <f>INDEX(z2nd,10)+Hght_WinWall1</f>
-        <v>4.58</v>
+        <v>7.0184000000000006</v>
       </c>
       <c r="J47" s="26">
         <f>INDEX(x3rd,9)</f>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="L47" s="26">
         <f>INDEX(z3rd,10)+Hght_WinWall1</f>
-        <v>7.6000000000000005</v>
+        <v>10.038399999999999</v>
       </c>
       <c r="N47" s="24">
         <v>0</v>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="P47" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
@@ -3803,7 +3803,7 @@
       </c>
       <c r="D48" s="29">
         <f>INDEX(z1st,2)+0.5</f>
-        <v>0.5</v>
+        <v>2.9384000000000001</v>
       </c>
       <c r="F48" s="28">
         <f>INDEX(x2nd,2)</f>
@@ -3815,7 +3815,7 @@
       </c>
       <c r="H48" s="29">
         <f>INDEX(z2nd,2)+0.5</f>
-        <v>3.22</v>
+        <v>5.6584000000000003</v>
       </c>
       <c r="J48" s="28">
         <f>INDEX(x3rd,2)</f>
@@ -3827,7 +3827,7 @@
       </c>
       <c r="L48" s="29">
         <f>INDEX(z3rd,2)+0.5</f>
-        <v>6.24</v>
+        <v>8.6783999999999999</v>
       </c>
       <c r="N48" s="25">
         <f>Opt_Width</f>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="P48" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -3855,7 +3855,7 @@
       </c>
       <c r="D49" s="29">
         <f>INDEX(z1st,3)+0.5</f>
-        <v>0.5</v>
+        <v>2.9384000000000001</v>
       </c>
       <c r="F49" s="28">
         <f>INDEX(x2nd,3)</f>
@@ -3867,7 +3867,7 @@
       </c>
       <c r="H49" s="29">
         <f>INDEX(z2nd,3)+0.5</f>
-        <v>3.22</v>
+        <v>5.6584000000000003</v>
       </c>
       <c r="J49" s="28">
         <f>INDEX(x3rd,3)</f>
@@ -3879,7 +3879,7 @@
       </c>
       <c r="L49" s="29">
         <f>INDEX(z3rd,3)+0.5</f>
-        <v>6.24</v>
+        <v>8.6783999999999999</v>
       </c>
       <c r="N49" s="25">
         <f>Opt_Width</f>
@@ -3891,7 +3891,7 @@
       </c>
       <c r="P49" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -3908,7 +3908,7 @@
       </c>
       <c r="D50" s="29">
         <f>INDEX(z1st,13)+Hght_WinWall2</f>
-        <v>1.86</v>
+        <v>4.2984</v>
       </c>
       <c r="F50" s="28">
         <f>INDEX(x2nd,7)</f>
@@ -3920,7 +3920,7 @@
       </c>
       <c r="H50" s="29">
         <f>INDEX(z2nd,13)+Hght_WinWall2</f>
-        <v>4.58</v>
+        <v>7.0184000000000006</v>
       </c>
       <c r="J50" s="28">
         <f>INDEX(x3rd,7)</f>
@@ -3932,7 +3932,7 @@
       </c>
       <c r="L50" s="29">
         <f>INDEX(z3rd,13)+Hght_WinWall2</f>
-        <v>7.6000000000000005</v>
+        <v>10.038399999999999</v>
       </c>
       <c r="N50" s="24">
         <v>0</v>
@@ -3943,7 +3943,7 @@
       </c>
       <c r="P50" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>8.51</v>
+        <v>10.948399999999999</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -3960,7 +3960,7 @@
       </c>
       <c r="D51" s="29">
         <f>INDEX(z1st,14)+Hght_WinWall2</f>
-        <v>1.86</v>
+        <v>4.2984</v>
       </c>
       <c r="F51" s="28">
         <f>INDEX(x2nd,6)</f>
@@ -3972,7 +3972,7 @@
       </c>
       <c r="H51" s="29">
         <f>INDEX(z2nd,14)+Hght_WinWall2</f>
-        <v>4.58</v>
+        <v>7.0184000000000006</v>
       </c>
       <c r="J51" s="28">
         <f>INDEX(x3rd,6)</f>
@@ -3984,7 +3984,7 @@
       </c>
       <c r="L51" s="29">
         <f>INDEX(z3rd,14)+Hght_WinWall2</f>
-        <v>7.6000000000000005</v>
+        <v>10.038399999999999</v>
       </c>
       <c r="N51" s="25">
         <f>+Opt_Roof_Peak_W</f>
@@ -4012,7 +4012,7 @@
       </c>
       <c r="D52" s="31">
         <f>INDEX(z1st,3)+0.5</f>
-        <v>0.5</v>
+        <v>2.9384000000000001</v>
       </c>
       <c r="F52" s="30">
         <f>INDEX(x2nd,3)-0.5</f>
@@ -4024,7 +4024,7 @@
       </c>
       <c r="H52" s="31">
         <f>INDEX(z2nd,3)+0.5</f>
-        <v>3.22</v>
+        <v>5.6584000000000003</v>
       </c>
       <c r="J52" s="30">
         <f>INDEX(x3rd,3)-0.5</f>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="L52" s="31">
         <f>INDEX(z3rd,3)+0.5</f>
-        <v>6.24</v>
+        <v>8.6783999999999999</v>
       </c>
       <c r="N52" s="25">
         <f>+Opt_Roof_Peak_W</f>
@@ -4065,7 +4065,7 @@
       </c>
       <c r="D53" s="31">
         <f>INDEX(z1st,4)+0.5</f>
-        <v>0.5</v>
+        <v>2.9384000000000001</v>
       </c>
       <c r="F53" s="30">
         <f>INDEX(x2nd,17)-Len_WinWall3</f>
@@ -4077,7 +4077,7 @@
       </c>
       <c r="H53" s="31">
         <f>INDEX(z2nd,4)+0.5</f>
-        <v>3.22</v>
+        <v>5.6584000000000003</v>
       </c>
       <c r="J53" s="30">
         <f>INDEX(x3rd,17)-Len_WinWall3</f>
@@ -4089,7 +4089,7 @@
       </c>
       <c r="L53" s="31">
         <f>INDEX(z3rd,4)+0.5</f>
-        <v>6.24</v>
+        <v>8.6783999999999999</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -4106,7 +4106,7 @@
       </c>
       <c r="D54" s="31">
         <f>INDEX(z1st,18)+Hght_WinWall3</f>
-        <v>1.86</v>
+        <v>4.2984</v>
       </c>
       <c r="F54" s="30">
         <f>INDEX(x2nd,18)</f>
@@ -4118,7 +4118,7 @@
       </c>
       <c r="H54" s="31">
         <f>INDEX(z2nd,18)+Hght_WinWall3</f>
-        <v>4.58</v>
+        <v>7.0184000000000006</v>
       </c>
       <c r="J54" s="30">
         <f>INDEX(x3rd,18)</f>
@@ -4130,7 +4130,7 @@
       </c>
       <c r="L54" s="31">
         <f>INDEX(z3rd,18)+Hght_WinWall3</f>
-        <v>7.6000000000000005</v>
+        <v>10.038399999999999</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -4147,7 +4147,7 @@
       </c>
       <c r="D55" s="31">
         <f>INDEX(z1st,19)</f>
-        <v>1.86</v>
+        <v>4.2984</v>
       </c>
       <c r="F55" s="30">
         <f>INDEX(x2nd,17)</f>
@@ -4159,7 +4159,7 @@
       </c>
       <c r="H55" s="31">
         <f>INDEX(z2nd,19)</f>
-        <v>4.58</v>
+        <v>7.0184000000000006</v>
       </c>
       <c r="J55" s="30">
         <f>INDEX(x3rd,17)</f>
@@ -4171,7 +4171,7 @@
       </c>
       <c r="L55" s="31">
         <f>INDEX(z3rd,19)</f>
-        <v>7.6000000000000005</v>
+        <v>10.038399999999999</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="D56" s="32">
         <f>INDEX(z1st,4)+0.5</f>
-        <v>0.5</v>
+        <v>2.9384000000000001</v>
       </c>
       <c r="F56" s="32">
         <f>INDEX(x2nd,4)</f>
@@ -4200,7 +4200,7 @@
       </c>
       <c r="H56" s="32">
         <f>INDEX(z2nd,4)+0.5</f>
-        <v>3.22</v>
+        <v>5.6584000000000003</v>
       </c>
       <c r="J56" s="32">
         <f>INDEX(x3rd,4)</f>
@@ -4212,7 +4212,7 @@
       </c>
       <c r="L56" s="32">
         <f>INDEX(z3rd,4)+0.5</f>
-        <v>6.24</v>
+        <v>8.6783999999999999</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -4229,7 +4229,7 @@
       </c>
       <c r="D57" s="32">
         <f>INDEX(z1st,1)+0.5</f>
-        <v>0.5</v>
+        <v>2.9384000000000001</v>
       </c>
       <c r="F57" s="32">
         <f>INDEX(x2nd,1)</f>
@@ -4241,7 +4241,7 @@
       </c>
       <c r="H57" s="32">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>3.22</v>
+        <v>5.6584000000000003</v>
       </c>
       <c r="J57" s="32">
         <f>INDEX(x3rd,1)</f>
@@ -4253,7 +4253,7 @@
       </c>
       <c r="L57" s="32">
         <f>INDEX(z3rd,1)+0.5</f>
-        <v>6.24</v>
+        <v>8.6783999999999999</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -4270,7 +4270,7 @@
       </c>
       <c r="D58" s="32">
         <f>INDEX(z1st,22)+Hght_WinWall4</f>
-        <v>1.86</v>
+        <v>4.2984</v>
       </c>
       <c r="F58" s="32">
         <f>INDEX(x2nd,5)</f>
@@ -4282,7 +4282,7 @@
       </c>
       <c r="H58" s="32">
         <f>INDEX(z2nd,22)+Hght_WinWall4</f>
-        <v>4.58</v>
+        <v>7.0184000000000006</v>
       </c>
       <c r="J58" s="32">
         <f>INDEX(x3rd,5)</f>
@@ -4294,7 +4294,7 @@
       </c>
       <c r="L58" s="32">
         <f>INDEX(z3rd,22)+Hght_WinWall4</f>
-        <v>7.6000000000000005</v>
+        <v>10.038399999999999</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -4311,7 +4311,7 @@
       </c>
       <c r="D59" s="32">
         <f>INDEX(z1st,23)</f>
-        <v>1.86</v>
+        <v>4.2984</v>
       </c>
       <c r="F59" s="32">
         <f>INDEX(x2nd,8)</f>
@@ -4323,7 +4323,7 @@
       </c>
       <c r="H59" s="32">
         <f>INDEX(z2nd,23)</f>
-        <v>4.58</v>
+        <v>7.0184000000000006</v>
       </c>
       <c r="J59" s="32">
         <f>INDEX(x3rd,8)</f>
@@ -4335,7 +4335,7 @@
       </c>
       <c r="L59" s="32">
         <f>INDEX(z3rd,23)</f>
-        <v>7.6000000000000005</v>
+        <v>10.038399999999999</v>
       </c>
     </row>
   </sheetData>
@@ -4728,15 +4728,15 @@
       </c>
       <c r="E21" s="55">
         <f>found_wall_area</f>
-        <v>0</v>
+        <v>77.81869489230769</v>
       </c>
       <c r="F21" s="55">
         <f>+E21*10.7639</f>
-        <v>0</v>
+        <v>837.63264995131067</v>
       </c>
       <c r="G21" s="68">
         <f>+F21*D21</f>
-        <v>0</v>
+        <v>3652.0783537877141</v>
       </c>
       <c r="H21" t="s">
         <v>173</v>
@@ -4783,15 +4783,15 @@
       </c>
       <c r="E24" s="55">
         <f>found_wall_area</f>
-        <v>0</v>
+        <v>77.81869489230769</v>
       </c>
       <c r="F24" s="55">
         <f>+E24*10.7639</f>
-        <v>0</v>
+        <v>837.63264995131067</v>
       </c>
       <c r="G24" s="68">
         <f>+F24*D24</f>
-        <v>0</v>
+        <v>7454.9305845666668</v>
       </c>
       <c r="H24" t="s">
         <v>174</v>

</xml_diff>